<commit_message>
Modify definition of runoff parameter
Part of #1.
</commit_message>
<xml_diff>
--- a/notebooks/input_template_critical_loads_water.xlsx
+++ b/notebooks/input_template_critical_loads_water.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Kari_A\Critical_Loads\new_workflow_nov_2018\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Kari_A\Critical_Loads\new_workflow_nov_2018\python\critical_loads_2\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DBAC11-6517-423C-9EBB-84E8A8FF7957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59B91BD-EEDE-4683-B412-6641D01FE3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{BF3CA8B3-4559-477A-99D2-75BE5B33240D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{BF3CA8B3-4559-477A-99D2-75BE5B33240D}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>Runoff</t>
   </si>
   <si>
-    <t>Average runoff over period 1960 to 1990</t>
-  </si>
-  <si>
     <t>Water chemistry concentration. Sulphate as SO4</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Unique identifier for region/catchment/site</t>
+  </si>
+  <si>
+    <t>Long-term average runoff</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CB183E-5103-4562-BF66-120F9FB1E320}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -802,9 +802,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513081C-F214-4FFD-9168-EB129EDD60F2}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -845,12 +845,12 @@
         <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -935,7 +935,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -952,7 +952,7 @@
         <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1020,7 +1020,7 @@
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1179,7 +1179,7 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <v>0.1</v>
@@ -1196,7 +1196,7 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -1251,7 +1251,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1306,7 +1306,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -1343,7 +1343,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
@@ -1358,10 +1358,10 @@
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Apply sea-salt correction to Magic parameters
</commit_message>
<xml_diff>
--- a/notebooks/input_template_critical_loads_water.xlsx
+++ b/notebooks/input_template_critical_loads_water.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Kari_A\Critical_Loads\new_workflow_nov_2018\python\critical_loads_2\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59B91BD-EEDE-4683-B412-6641D01FE3CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB3A27C-42A1-47A8-9269-491858B000B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{BF3CA8B3-4559-477A-99D2-75BE5B33240D}"/>
   </bookViews>
@@ -20,9 +20,9 @@
     <sheet name="optional_parameters" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">magic_parameters!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">magic_parameters!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">optional_parameters!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameter_definitions!$A$1:$F$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameter_definitions!$A$1:$F$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">required_parameters!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
   <si>
     <t>Ca</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Long-term average runoff</t>
+  </si>
+  <si>
+    <t>Cl_magic</t>
   </si>
 </sst>
 </file>
@@ -800,11 +803,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513081C-F214-4FFD-9168-EB129EDD60F2}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1096,19 +1099,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1119,16 +1119,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1139,16 +1139,16 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
       <c r="E19">
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1159,16 +1159,16 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E20">
-        <v>3.57</v>
+        <v>0.95</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1179,13 +1179,16 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
       </c>
       <c r="E21">
-        <v>0.1</v>
+        <v>3.57</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -1196,16 +1199,13 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1216,20 +1216,40 @@
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
       </c>
       <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24">
         <v>0.5</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F23" xr:uid="{A0099389-6DB9-430C-96BD-F630BFBF6D3F}"/>
+  <autoFilter ref="A1:F24" xr:uid="{A0099389-6DB9-430C-96BD-F630BFBF6D3F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1292,19 +1312,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454EF675-CC3A-4D29-840B-3B11A946E4D6}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="5" width="13.73046875" customWidth="1"/>
+    <col min="6" max="6" width="10.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1320,9 +1341,12 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{1976CB1D-2E83-429E-984A-9959F2A87095}"/>
+  <autoFilter ref="A1:F1" xr:uid="{67B93750-BC0C-4B1C-AFEC-AD180C17155C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>